<commit_message>
Added microcontroller and FTDI chip for analysis
</commit_message>
<xml_diff>
--- a/Power Analysis.xlsx
+++ b/Power Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckeer\Documents\GitHub\pathfinder_payload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1257BB1-DA93-43B8-80DC-ECF9CD47438C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA20D2E2-DFB2-43CA-BC94-710E1861A104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D8327CE6-015E-4803-AF5C-CE15EE058163}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Part (name)</t>
   </si>
@@ -52,16 +52,39 @@
   </si>
   <si>
     <t>AtMega328P-AU</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/ATMEGA328P-AU/ATMEGA328P-AU-ND/1832260</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>16 MHz Crystal</t>
+  </si>
+  <si>
+    <t>FT232RL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/ftdi-future-technology-devices-international-ltd/FT232RL-REEL/768-1007-1-ND/1836402</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,13 +107,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED81A6F-8573-421B-8CB2-07EDB74F646E}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,9 +442,10 @@
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,13 +461,48 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0.02</v>
+      </c>
+      <c r="D2">
+        <v>0.02</v>
+      </c>
+      <c r="E2">
+        <v>0.06</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{8E6BA5B5-5FFC-4D0F-A6E1-90FED8D6B251}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{50663E31-54F6-4D48-8CBF-F29D1F728DD4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>